<commit_message>
Projecting up to 2100
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230912.xlsx
+++ b/data/hake_intrasp_230912.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{194303BD-444B-624C-9B13-C0C86EF31E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA30D5-35D0-EC41-9FAB-7AFABA75D9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21648,7 +21648,7 @@
         <v>21</v>
       </c>
       <c r="B5">
-        <v>2050</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>